<commit_message>
Se actulizo la interpretacion de rutas absolutas a relativas
</commit_message>
<xml_diff>
--- a/pipelines/full_consolidated_inventory.xlsx
+++ b/pipelines/full_consolidated_inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/195e9c5e92fd952e/Documents/ALGO TRADING/SP500_INDEX_Analisis/pipelines/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{AF728CD0-D43A-4526-B750-3634CD44010D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF3CDEBF-FAD3-4DF0-8E9B-8E71B605CB17}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F6C12A-468B-41EA-A20A-F322D21339F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="118">
   <si>
     <t>instrument</t>
   </si>
@@ -173,33 +173,6 @@
     <t>JPY_USD_Spot.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\index_pricing\S&amp;P500_Index.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\index_pricing\VIX_VolatilityIndex.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\bond\US_10Y_Treasury.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\economics\US_FedFunds_Rate.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\economics\US_CPI.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\commodities\CrudeOil_WTI.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\unemployment_rate\US_Unemployment_Rate.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\exchange_rate\EUR_USD_Spot.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\exchange_rate\JPY_USD_Spot.csv</t>
-  </si>
-  <si>
     <t>time_index</t>
   </si>
   <si>
@@ -230,18 +203,12 @@
     <t>US_ISM_Manufacturing.xlsx</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\business_confidence\US_ISM_Manufacturing.xlsx</t>
-  </si>
-  <si>
     <t>michigan_sentiment_raw</t>
   </si>
   <si>
     <t>Michigan_Consumer_Sentiment.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\consumer_confidence\Michigan_Consumer_Sentiment.csv</t>
-  </si>
-  <si>
     <t>SARIMAX_EXTENDED</t>
   </si>
   <si>
@@ -272,18 +239,12 @@
     <t>Dollar_Index_DXY.xlsx</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\index_pricing\Dollar_Index_DXY.xlsx</t>
-  </si>
-  <si>
     <t>ecb_rate</t>
   </si>
   <si>
     <t>ECB_Deposit_Rate.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\economics\ECB_Deposit_Rate.csv</t>
-  </si>
-  <si>
     <t>fed_funds</t>
   </si>
   <si>
@@ -293,9 +254,6 @@
     <t>Eurozone_Unemployment_Rate.xlsx</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\unemployment_rate\Eurozone_Unemployment_Rate.xlsx</t>
-  </si>
-  <si>
     <t>us_unemployment_raw</t>
   </si>
   <si>
@@ -305,9 +263,6 @@
     <t>EuroZone_Consumer_Confidence.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\consumer_confidence\EuroZone_Consumer_Confidence.csv</t>
-  </si>
-  <si>
     <t>usdjpy_open</t>
   </si>
   <si>
@@ -326,36 +281,24 @@
     <t>BOJ_Policy_Rate.xlsx</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\economics\BOJ_Policy_Rate.xlsx</t>
-  </si>
-  <si>
     <t>japan_leading_indicator_raw</t>
   </si>
   <si>
     <t>Japan_Leading_Indicator.xlsx</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\leading_economic_index\Japan_Leading_Indicator.xlsx</t>
-  </si>
-  <si>
     <t>nikkei_225_raw</t>
   </si>
   <si>
     <t>Nikkei_225.csv</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\index_pricing\Nikkei_225.csv</t>
-  </si>
-  <si>
     <t>japan_m2_raw</t>
   </si>
   <si>
     <t>Japan_M2_MoneySupply_YoY.xlsx</t>
   </si>
   <si>
-    <t>C:\Users\pedro\OneDrive\Documents\ALGO TRADING\SP500_INDEX_Analisis\data\0_raw\economics\Japan_M2_MoneySupply_YoY.xlsx</t>
-  </si>
-  <si>
     <t>ARIMA|SARIMAX_BASIC|SARIMAX_EXTENDED</t>
   </si>
   <si>
@@ -387,6 +330,66 @@
   </si>
   <si>
     <t>CSCICP02EZM460S</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\index_pricing\S&amp;P500_Index.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\index_pricing\VIX_VolatilityIndex.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\bond\US_10Y_Treasury.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\economics\US_FedFunds_Rate.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\economics\US_CPI.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\commodities\CrudeOil_WTI.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\unemployment_rate\US_Unemployment_Rate.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\business_confidence\US_ISM_Manufacturing.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\consumer_confidence\Michigan_Consumer_Sentiment.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\exchange_rate\EUR_USD_Spot.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\index_pricing\Dollar_Index_DXY.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\economics\ECB_Deposit_Rate.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\unemployment_rate\Eurozone_Unemployment_Rate.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\consumer_confidence\EuroZone_Consumer_Confidence.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\exchange_rate\JPY_USD_Spot.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\economics\BOJ_Policy_Rate.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\leading_economic_index\Japan_Leading_Indicator.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\index_pricing\Nikkei_225.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\economics\Japan_M2_MoneySupply_YoY.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\SP500_INDEX_Analisis\data\0_raw\index_pricing\S&amp;P500_Index.csv</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -454,6 +457,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,7 +769,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="F40" sqref="A40:XFD48"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,6 +781,7 @@
     <col min="7" max="7" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="133.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="56.109375" bestFit="1" customWidth="1"/>
@@ -790,13 +795,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -828,7 +833,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3">
         <f>IF(B2="ARIMA|SARIMAX_BASIC|SARIMAX_EXTENDED",1,0)</f>
@@ -851,14 +856,14 @@
       <c r="H2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L2" s="3">
         <v>0</v>
@@ -870,7 +875,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C3" s="3">
         <f t="shared" ref="C3:C39" si="0">IF(B3="ARIMA|SARIMAX_BASIC|SARIMAX_EXTENDED",1,0)</f>
@@ -894,13 +899,13 @@
         <v>36</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="L3" s="3">
         <v>0</v>
@@ -912,7 +917,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" si="0"/>
@@ -936,13 +941,13 @@
         <v>36</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L4" s="3">
         <v>0</v>
@@ -954,7 +959,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" si="0"/>
@@ -978,13 +983,13 @@
         <v>36</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L5" s="3">
         <v>0</v>
@@ -996,7 +1001,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" si="0"/>
@@ -1020,13 +1025,13 @@
         <v>36</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L6" s="3">
         <v>0</v>
@@ -1062,13 +1067,13 @@
         <v>36</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L7" s="3">
         <v>0</v>
@@ -1104,13 +1109,13 @@
         <v>37</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L8" s="3">
         <v>0</v>
@@ -1140,19 +1145,19 @@
         <v>21</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L9" s="3">
         <v>0</v>
@@ -1182,19 +1187,19 @@
         <v>22</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L10" s="3">
         <v>0</v>
@@ -1224,19 +1229,19 @@
         <v>23</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>40</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L11" s="3">
         <v>14</v>
@@ -1272,13 +1277,13 @@
         <v>41</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L12" s="3">
         <v>0</v>
@@ -1308,19 +1313,19 @@
         <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>42</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L13" s="3">
         <v>3</v>
@@ -1332,7 +1337,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" si="0"/>
@@ -1347,22 +1352,22 @@
         <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L14" s="3">
         <v>3</v>
@@ -1374,7 +1379,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="0"/>
@@ -1389,22 +1394,22 @@
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L15" s="3">
         <v>14</v>
@@ -1416,7 +1421,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="0"/>
@@ -1440,13 +1445,13 @@
         <v>43</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L16" s="3">
         <v>0</v>
@@ -1458,7 +1463,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="0"/>
@@ -1482,13 +1487,13 @@
         <v>43</v>
       </c>
       <c r="I17" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="L17" s="3">
         <v>0</v>
@@ -1500,7 +1505,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C18" s="3">
         <f t="shared" si="0"/>
@@ -1515,22 +1520,22 @@
         <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>43</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L18" s="3">
         <v>0</v>
@@ -1542,7 +1547,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="0"/>
@@ -1557,22 +1562,22 @@
         <v>1</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>43</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L19" s="3">
         <v>0</v>
@@ -1584,7 +1589,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="0"/>
@@ -1599,22 +1604,22 @@
         <v>1</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>43</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L20" s="3">
         <v>0</v>
@@ -1641,7 +1646,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>33</v>
@@ -1650,13 +1655,13 @@
         <v>43</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L21" s="3">
         <v>0</v>
@@ -1683,22 +1688,22 @@
         <v>1</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>35</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L22" s="3">
         <v>0</v>
@@ -1725,22 +1730,22 @@
         <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L23" s="3">
         <v>0</v>
@@ -1767,22 +1772,22 @@
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I24" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J24" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="K24" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L24" s="3">
         <v>0</v>
@@ -1809,22 +1814,22 @@
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L25" s="3">
         <v>30</v>
@@ -1851,22 +1856,22 @@
         <v>1</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="G26" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>42</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L26" s="3">
         <v>3</v>
@@ -1878,7 +1883,7 @@
         <v>11</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C27" s="3">
         <f t="shared" si="0"/>
@@ -1893,22 +1898,22 @@
         <v>1</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L27" s="3">
         <v>14</v>
@@ -1920,7 +1925,7 @@
         <v>12</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" si="0"/>
@@ -1944,13 +1949,13 @@
         <v>44</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L28" s="3">
         <v>0</v>
@@ -1962,7 +1967,7 @@
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="C29" s="3">
         <f t="shared" si="0"/>
@@ -1986,13 +1991,13 @@
         <v>44</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="L29" s="3">
         <v>0</v>
@@ -2004,7 +2009,7 @@
         <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" si="0"/>
@@ -2019,22 +2024,22 @@
         <v>1</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L30" s="3">
         <v>0</v>
@@ -2046,7 +2051,7 @@
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" si="0"/>
@@ -2061,22 +2066,22 @@
         <v>1</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L31" s="3">
         <v>0</v>
@@ -2088,7 +2093,7 @@
         <v>12</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" si="0"/>
@@ -2103,22 +2108,22 @@
         <v>1</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>44</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L32" s="3">
         <v>0</v>
@@ -2145,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>33</v>
@@ -2154,13 +2159,13 @@
         <v>44</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L33" s="3">
         <v>0</v>
@@ -2187,22 +2192,22 @@
         <v>1</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L34" s="3">
         <v>0</v>
@@ -2229,22 +2234,22 @@
         <v>1</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="H35" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J35" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="J35" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="K35" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L35" s="3">
         <v>0</v>
@@ -2271,22 +2276,22 @@
         <v>1</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="G36" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L36" s="3">
         <v>30</v>
@@ -2313,22 +2318,22 @@
         <v>1</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="G37" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>42</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L37" s="3">
         <v>3</v>
@@ -2355,22 +2360,22 @@
         <v>1</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="G38" t="s">
         <v>29</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L38" s="3">
         <v>0</v>
@@ -2382,7 +2387,7 @@
         <v>12</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C39" s="3">
         <f t="shared" si="0"/>
@@ -2397,22 +2402,22 @@
         <v>1</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="G39" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="L39" s="3">
         <v>14</v>
@@ -2422,5 +2427,6 @@
   </sheetData>
   <autoFilter ref="A1:M39" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revision mes de Abril
</commit_message>
<xml_diff>
--- a/pipelines/full_consolidated_inventory.xlsx
+++ b/pipelines/full_consolidated_inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\pipelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F6C12A-468B-41EA-A20A-F322D21339F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B11D04-8B47-4539-BADC-70AC40E3FE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="117">
   <si>
     <t>instrument</t>
   </si>
@@ -387,9 +387,6 @@
   </si>
   <si>
     <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\Proyecto_Mercado_de_Valores\SP500_INDEX_Analisis\data\0_raw\economics\Japan_M2_MoneySupply_YoY.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\natus\Documents\Trabajo\PEDRO_PEREZ\SP500_INDEX_Analisis\data\0_raw\index_pricing\S&amp;P500_Index.csv</t>
   </si>
 </sst>
 </file>
@@ -768,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -857,7 +854,7 @@
         <v>36</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>45</v>
@@ -898,7 +895,7 @@
       <c r="H3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>98</v>
       </c>
       <c r="J3" s="3" t="s">

</xml_diff>